<commit_message>
added finger vs nofinger perf results
</commit_message>
<xml_diff>
--- a/doc/diag/finger_performance.xlsx
+++ b/doc/diag/finger_performance.xlsx
@@ -165,10 +165,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet2!$I$2:$I$5</c:f>
+              <c:f>Sheet2!$I$2:$I$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -181,15 +181,18 @@
                 <c:pt idx="3">
                   <c:v>16</c:v>
                 </c:pt>
+                <c:pt idx="4">
+                  <c:v>32</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet2!$J$2:$J$5</c:f>
+              <c:f>Sheet2!$J$2:$J$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -202,6 +205,9 @@
                 <c:pt idx="3">
                   <c:v>7.5</c:v>
                 </c:pt>
+                <c:pt idx="4">
+                  <c:v>15.5</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -212,11 +218,11 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet2!$K$1</c:f>
+              <c:f>Sheet2!$K$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Fingers enabled</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -247,10 +253,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet2!$I$2:$I$5</c:f>
+              <c:f>Sheet2!$I$2:$I$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -263,15 +269,18 @@
                 <c:pt idx="3">
                   <c:v>16</c:v>
                 </c:pt>
+                <c:pt idx="4">
+                  <c:v>32</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet2!$K$2:$K$4</c:f>
+              <c:f>Sheet2!$K$2:$K$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -279,7 +288,13 @@
                   <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.1428571428571428</c:v>
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.75</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.375</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1145,13 +1160,13 @@
       <xdr:col>12</xdr:col>
       <xdr:colOff>38099</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:rowOff>47624</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>581024</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>171449</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1474,10 +1489,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M28"/>
+  <dimension ref="A1:M60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="Y40" sqref="Y40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1553,21 +1568,21 @@
         <v>7</v>
       </c>
       <c r="E3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F3">
         <f>AVERAGEIF($D$3:$D$100,D3,$E$3:$E$100)</f>
-        <v>2.1428571428571428</v>
+        <v>1</v>
       </c>
       <c r="I3">
         <v>2</v>
       </c>
       <c r="J3">
-        <f t="shared" ref="J3:J5" si="0">VLOOKUP(I3,$A$3:$C$100,3,FALSE)</f>
+        <f t="shared" ref="J3:J6" si="0">VLOOKUP(I3,$A$3:$C$100,3,FALSE)</f>
         <v>0.5</v>
       </c>
       <c r="K3">
-        <f t="shared" ref="K3:K5" si="1">VLOOKUP(I3,$D$3:$F$100,3,FALSE)</f>
+        <f t="shared" ref="K3:K6" si="1">VLOOKUP(I3,$D$3:$F$100,3,FALSE)</f>
         <v>0.5</v>
       </c>
     </row>
@@ -1579,18 +1594,18 @@
         <v>1</v>
       </c>
       <c r="C4">
-        <f t="shared" ref="C4:C28" si="2">AVERAGEIF($A$3:$A$100,A4,$B$3:$B$100)</f>
+        <f t="shared" ref="C4:C60" si="2">AVERAGEIF($A$3:$A$100,A4,$B$3:$B$100)</f>
         <v>3</v>
       </c>
       <c r="D4">
         <v>7</v>
       </c>
       <c r="E4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F4">
-        <f t="shared" ref="F4:F28" si="3">AVERAGEIF($D$3:$D$100,D4,$E$3:$E$100)</f>
-        <v>2.1428571428571428</v>
+        <f t="shared" ref="F4:F60" si="3">AVERAGEIF($D$3:$D$100,D4,$E$3:$E$100)</f>
+        <v>1</v>
       </c>
       <c r="I4">
         <v>7</v>
@@ -1601,7 +1616,7 @@
       </c>
       <c r="K4">
         <f t="shared" si="1"/>
-        <v>2.1428571428571428</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -1619,11 +1634,11 @@
         <v>7</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F5">
         <f t="shared" si="3"/>
-        <v>2.1428571428571428</v>
+        <v>1</v>
       </c>
       <c r="I5">
         <v>16</v>
@@ -1632,9 +1647,9 @@
         <f t="shared" si="0"/>
         <v>7.5</v>
       </c>
-      <c r="K5" t="e">
+      <c r="K5">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>1.75</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -1656,7 +1671,18 @@
       </c>
       <c r="F6">
         <f t="shared" si="3"/>
-        <v>2.1428571428571428</v>
+        <v>1</v>
+      </c>
+      <c r="I6">
+        <v>32</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="0"/>
+        <v>15.5</v>
+      </c>
+      <c r="K6">
+        <f t="shared" si="1"/>
+        <v>2.375</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -1674,11 +1700,11 @@
         <v>7</v>
       </c>
       <c r="E7">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F7">
         <f t="shared" si="3"/>
-        <v>2.1428571428571428</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
@@ -1696,11 +1722,11 @@
         <v>7</v>
       </c>
       <c r="E8">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F8">
         <f t="shared" si="3"/>
-        <v>2.1428571428571428</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
@@ -1718,11 +1744,11 @@
         <v>7</v>
       </c>
       <c r="E9">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F9">
         <f t="shared" si="3"/>
-        <v>2.1428571428571428</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
@@ -1805,9 +1831,12 @@
       <c r="D13">
         <v>16</v>
       </c>
-      <c r="F13" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+      <c r="E13">
+        <v>2</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="3"/>
+        <v>1.75</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
@@ -1824,9 +1853,12 @@
       <c r="D14">
         <v>16</v>
       </c>
-      <c r="F14" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+      <c r="E14">
+        <v>3</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="3"/>
+        <v>1.75</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
@@ -1843,9 +1875,12 @@
       <c r="D15">
         <v>16</v>
       </c>
-      <c r="F15" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="3"/>
+        <v>1.75</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
@@ -1862,9 +1897,12 @@
       <c r="D16">
         <v>16</v>
       </c>
-      <c r="F16" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+      <c r="E16">
+        <v>2</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="3"/>
+        <v>1.75</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -1881,9 +1919,12 @@
       <c r="D17">
         <v>16</v>
       </c>
-      <c r="F17" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+      <c r="E17">
+        <v>4</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="3"/>
+        <v>1.75</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -1900,9 +1941,12 @@
       <c r="D18">
         <v>16</v>
       </c>
-      <c r="F18" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+      <c r="E18">
+        <v>2</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="3"/>
+        <v>1.75</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -1919,9 +1963,12 @@
       <c r="D19">
         <v>16</v>
       </c>
-      <c r="F19" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+      <c r="E19">
+        <v>2</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="3"/>
+        <v>1.75</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -1938,9 +1985,12 @@
       <c r="D20">
         <v>16</v>
       </c>
-      <c r="F20" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+      <c r="E20">
+        <v>2</v>
+      </c>
+      <c r="F20">
+        <f t="shared" si="3"/>
+        <v>1.75</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -1957,9 +2007,12 @@
       <c r="D21">
         <v>16</v>
       </c>
-      <c r="F21" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+      <c r="E21">
+        <v>1</v>
+      </c>
+      <c r="F21">
+        <f t="shared" si="3"/>
+        <v>1.75</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -1976,9 +2029,12 @@
       <c r="D22">
         <v>16</v>
       </c>
-      <c r="F22" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+      <c r="E22">
+        <v>1</v>
+      </c>
+      <c r="F22">
+        <f t="shared" si="3"/>
+        <v>1.75</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -1995,9 +2051,12 @@
       <c r="D23">
         <v>16</v>
       </c>
-      <c r="F23" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+      <c r="E23">
+        <v>1</v>
+      </c>
+      <c r="F23">
+        <f t="shared" si="3"/>
+        <v>1.75</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -2014,9 +2073,12 @@
       <c r="D24">
         <v>16</v>
       </c>
-      <c r="F24" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+      <c r="E24">
+        <v>2</v>
+      </c>
+      <c r="F24">
+        <f t="shared" si="3"/>
+        <v>1.75</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -2033,9 +2095,12 @@
       <c r="D25">
         <v>16</v>
       </c>
-      <c r="F25" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+      <c r="E25">
+        <v>2</v>
+      </c>
+      <c r="F25">
+        <f t="shared" si="3"/>
+        <v>1.75</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -2052,9 +2117,12 @@
       <c r="D26">
         <v>16</v>
       </c>
-      <c r="F26" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+      <c r="E26">
+        <v>1</v>
+      </c>
+      <c r="F26">
+        <f t="shared" si="3"/>
+        <v>1.75</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -2071,9 +2139,12 @@
       <c r="D27">
         <v>16</v>
       </c>
-      <c r="F27" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+      <c r="E27">
+        <v>0</v>
+      </c>
+      <c r="F27">
+        <f t="shared" si="3"/>
+        <v>1.75</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -2090,9 +2161,716 @@
       <c r="D28">
         <v>16</v>
       </c>
-      <c r="F28" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+      <c r="E28">
+        <v>2</v>
+      </c>
+      <c r="F28">
+        <f t="shared" si="3"/>
+        <v>1.75</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>32</v>
+      </c>
+      <c r="B29">
+        <v>0</v>
+      </c>
+      <c r="C29">
+        <f t="shared" si="2"/>
+        <v>15.5</v>
+      </c>
+      <c r="D29">
+        <v>32</v>
+      </c>
+      <c r="E29">
+        <v>3</v>
+      </c>
+      <c r="F29">
+        <f t="shared" si="3"/>
+        <v>2.375</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>32</v>
+      </c>
+      <c r="B30">
+        <v>1</v>
+      </c>
+      <c r="C30">
+        <f t="shared" si="2"/>
+        <v>15.5</v>
+      </c>
+      <c r="D30">
+        <v>32</v>
+      </c>
+      <c r="E30">
+        <v>3</v>
+      </c>
+      <c r="F30">
+        <f t="shared" si="3"/>
+        <v>2.375</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>32</v>
+      </c>
+      <c r="B31">
+        <v>2</v>
+      </c>
+      <c r="C31">
+        <f t="shared" si="2"/>
+        <v>15.5</v>
+      </c>
+      <c r="D31">
+        <v>32</v>
+      </c>
+      <c r="E31">
+        <v>2</v>
+      </c>
+      <c r="F31">
+        <f t="shared" si="3"/>
+        <v>2.375</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>32</v>
+      </c>
+      <c r="B32">
+        <v>3</v>
+      </c>
+      <c r="C32">
+        <f t="shared" si="2"/>
+        <v>15.5</v>
+      </c>
+      <c r="D32">
+        <v>32</v>
+      </c>
+      <c r="E32">
+        <v>4</v>
+      </c>
+      <c r="F32">
+        <f t="shared" si="3"/>
+        <v>2.375</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33">
+        <v>4</v>
+      </c>
+      <c r="C33">
+        <f t="shared" si="2"/>
+        <v>15.5</v>
+      </c>
+      <c r="D33">
+        <v>32</v>
+      </c>
+      <c r="E33">
+        <v>2</v>
+      </c>
+      <c r="F33">
+        <f t="shared" si="3"/>
+        <v>2.375</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>32</v>
+      </c>
+      <c r="B34">
+        <v>5</v>
+      </c>
+      <c r="C34">
+        <f t="shared" si="2"/>
+        <v>15.5</v>
+      </c>
+      <c r="D34">
+        <v>32</v>
+      </c>
+      <c r="E34">
+        <v>2</v>
+      </c>
+      <c r="F34">
+        <f t="shared" si="3"/>
+        <v>2.375</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>32</v>
+      </c>
+      <c r="B35">
+        <v>6</v>
+      </c>
+      <c r="C35">
+        <f t="shared" si="2"/>
+        <v>15.5</v>
+      </c>
+      <c r="D35">
+        <v>32</v>
+      </c>
+      <c r="E35">
+        <v>2</v>
+      </c>
+      <c r="F35">
+        <f t="shared" si="3"/>
+        <v>2.375</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>32</v>
+      </c>
+      <c r="B36">
+        <v>7</v>
+      </c>
+      <c r="C36">
+        <f t="shared" si="2"/>
+        <v>15.5</v>
+      </c>
+      <c r="D36">
+        <v>32</v>
+      </c>
+      <c r="E36">
+        <v>2</v>
+      </c>
+      <c r="F36">
+        <f t="shared" si="3"/>
+        <v>2.375</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>32</v>
+      </c>
+      <c r="B37">
+        <v>8</v>
+      </c>
+      <c r="C37">
+        <f t="shared" si="2"/>
+        <v>15.5</v>
+      </c>
+      <c r="D37">
+        <v>32</v>
+      </c>
+      <c r="E37">
+        <v>3</v>
+      </c>
+      <c r="F37">
+        <f t="shared" si="3"/>
+        <v>2.375</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>32</v>
+      </c>
+      <c r="B38">
+        <v>9</v>
+      </c>
+      <c r="C38">
+        <f t="shared" si="2"/>
+        <v>15.5</v>
+      </c>
+      <c r="D38">
+        <v>32</v>
+      </c>
+      <c r="E38">
+        <v>1</v>
+      </c>
+      <c r="F38">
+        <f t="shared" si="3"/>
+        <v>2.375</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>32</v>
+      </c>
+      <c r="B39">
+        <v>10</v>
+      </c>
+      <c r="C39">
+        <f t="shared" si="2"/>
+        <v>15.5</v>
+      </c>
+      <c r="D39">
+        <v>32</v>
+      </c>
+      <c r="E39">
+        <v>2</v>
+      </c>
+      <c r="F39">
+        <f t="shared" si="3"/>
+        <v>2.375</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>32</v>
+      </c>
+      <c r="B40">
+        <v>11</v>
+      </c>
+      <c r="C40">
+        <f t="shared" si="2"/>
+        <v>15.5</v>
+      </c>
+      <c r="D40">
+        <v>32</v>
+      </c>
+      <c r="E40">
+        <v>3</v>
+      </c>
+      <c r="F40">
+        <f t="shared" si="3"/>
+        <v>2.375</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>32</v>
+      </c>
+      <c r="B41">
+        <v>12</v>
+      </c>
+      <c r="C41">
+        <f t="shared" si="2"/>
+        <v>15.5</v>
+      </c>
+      <c r="D41">
+        <v>32</v>
+      </c>
+      <c r="E41">
+        <v>3</v>
+      </c>
+      <c r="F41">
+        <f t="shared" si="3"/>
+        <v>2.375</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>32</v>
+      </c>
+      <c r="B42">
+        <v>13</v>
+      </c>
+      <c r="C42">
+        <f t="shared" si="2"/>
+        <v>15.5</v>
+      </c>
+      <c r="D42">
+        <v>32</v>
+      </c>
+      <c r="E42">
+        <v>2</v>
+      </c>
+      <c r="F42">
+        <f t="shared" si="3"/>
+        <v>2.375</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>32</v>
+      </c>
+      <c r="B43">
+        <v>14</v>
+      </c>
+      <c r="C43">
+        <f t="shared" si="2"/>
+        <v>15.5</v>
+      </c>
+      <c r="D43">
+        <v>32</v>
+      </c>
+      <c r="E43">
+        <v>2</v>
+      </c>
+      <c r="F43">
+        <f t="shared" si="3"/>
+        <v>2.375</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>32</v>
+      </c>
+      <c r="B44">
+        <v>15</v>
+      </c>
+      <c r="C44">
+        <f t="shared" si="2"/>
+        <v>15.5</v>
+      </c>
+      <c r="D44">
+        <v>32</v>
+      </c>
+      <c r="E44">
+        <v>3</v>
+      </c>
+      <c r="F44">
+        <f t="shared" si="3"/>
+        <v>2.375</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>32</v>
+      </c>
+      <c r="B45">
+        <v>16</v>
+      </c>
+      <c r="C45">
+        <f t="shared" si="2"/>
+        <v>15.5</v>
+      </c>
+      <c r="D45">
+        <v>32</v>
+      </c>
+      <c r="E45">
+        <v>3</v>
+      </c>
+      <c r="F45">
+        <f t="shared" si="3"/>
+        <v>2.375</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>32</v>
+      </c>
+      <c r="B46">
+        <v>17</v>
+      </c>
+      <c r="C46">
+        <f t="shared" si="2"/>
+        <v>15.5</v>
+      </c>
+      <c r="D46">
+        <v>32</v>
+      </c>
+      <c r="E46">
+        <v>3</v>
+      </c>
+      <c r="F46">
+        <f t="shared" si="3"/>
+        <v>2.375</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>32</v>
+      </c>
+      <c r="B47">
+        <v>18</v>
+      </c>
+      <c r="C47">
+        <f t="shared" si="2"/>
+        <v>15.5</v>
+      </c>
+      <c r="D47">
+        <v>32</v>
+      </c>
+      <c r="E47">
+        <v>1</v>
+      </c>
+      <c r="F47">
+        <f t="shared" si="3"/>
+        <v>2.375</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>32</v>
+      </c>
+      <c r="B48">
+        <v>19</v>
+      </c>
+      <c r="C48">
+        <f t="shared" si="2"/>
+        <v>15.5</v>
+      </c>
+      <c r="D48">
+        <v>32</v>
+      </c>
+      <c r="E48">
+        <v>1</v>
+      </c>
+      <c r="F48">
+        <f t="shared" si="3"/>
+        <v>2.375</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>32</v>
+      </c>
+      <c r="B49">
+        <v>20</v>
+      </c>
+      <c r="C49">
+        <f t="shared" si="2"/>
+        <v>15.5</v>
+      </c>
+      <c r="D49">
+        <v>32</v>
+      </c>
+      <c r="E49">
+        <v>3</v>
+      </c>
+      <c r="F49">
+        <f t="shared" si="3"/>
+        <v>2.375</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>32</v>
+      </c>
+      <c r="B50">
+        <v>21</v>
+      </c>
+      <c r="C50">
+        <f t="shared" si="2"/>
+        <v>15.5</v>
+      </c>
+      <c r="D50">
+        <v>32</v>
+      </c>
+      <c r="E50">
+        <v>2</v>
+      </c>
+      <c r="F50">
+        <f t="shared" si="3"/>
+        <v>2.375</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>32</v>
+      </c>
+      <c r="B51">
+        <v>22</v>
+      </c>
+      <c r="C51">
+        <f t="shared" si="2"/>
+        <v>15.5</v>
+      </c>
+      <c r="D51">
+        <v>32</v>
+      </c>
+      <c r="E51">
+        <v>3</v>
+      </c>
+      <c r="F51">
+        <f t="shared" si="3"/>
+        <v>2.375</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>32</v>
+      </c>
+      <c r="B52">
+        <v>23</v>
+      </c>
+      <c r="C52">
+        <f t="shared" si="2"/>
+        <v>15.5</v>
+      </c>
+      <c r="D52">
+        <v>32</v>
+      </c>
+      <c r="E52">
+        <v>2</v>
+      </c>
+      <c r="F52">
+        <f t="shared" si="3"/>
+        <v>2.375</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>32</v>
+      </c>
+      <c r="B53">
+        <v>24</v>
+      </c>
+      <c r="C53">
+        <f t="shared" si="2"/>
+        <v>15.5</v>
+      </c>
+      <c r="D53">
+        <v>32</v>
+      </c>
+      <c r="E53">
+        <v>3</v>
+      </c>
+      <c r="F53">
+        <f t="shared" si="3"/>
+        <v>2.375</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>32</v>
+      </c>
+      <c r="B54">
+        <v>25</v>
+      </c>
+      <c r="C54">
+        <f t="shared" si="2"/>
+        <v>15.5</v>
+      </c>
+      <c r="D54">
+        <v>32</v>
+      </c>
+      <c r="E54">
+        <v>2</v>
+      </c>
+      <c r="F54">
+        <f t="shared" si="3"/>
+        <v>2.375</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>32</v>
+      </c>
+      <c r="B55">
+        <v>26</v>
+      </c>
+      <c r="C55">
+        <f t="shared" si="2"/>
+        <v>15.5</v>
+      </c>
+      <c r="D55">
+        <v>32</v>
+      </c>
+      <c r="E55">
+        <v>3</v>
+      </c>
+      <c r="F55">
+        <f t="shared" si="3"/>
+        <v>2.375</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>32</v>
+      </c>
+      <c r="B56">
+        <v>27</v>
+      </c>
+      <c r="C56">
+        <f t="shared" si="2"/>
+        <v>15.5</v>
+      </c>
+      <c r="D56">
+        <v>32</v>
+      </c>
+      <c r="E56">
+        <v>3</v>
+      </c>
+      <c r="F56">
+        <f t="shared" si="3"/>
+        <v>2.375</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>32</v>
+      </c>
+      <c r="B57">
+        <v>28</v>
+      </c>
+      <c r="C57">
+        <f t="shared" si="2"/>
+        <v>15.5</v>
+      </c>
+      <c r="D57">
+        <v>32</v>
+      </c>
+      <c r="E57">
+        <v>3</v>
+      </c>
+      <c r="F57">
+        <f t="shared" si="3"/>
+        <v>2.375</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>32</v>
+      </c>
+      <c r="B58">
+        <v>29</v>
+      </c>
+      <c r="C58">
+        <f t="shared" si="2"/>
+        <v>15.5</v>
+      </c>
+      <c r="D58">
+        <v>32</v>
+      </c>
+      <c r="E58">
+        <v>3</v>
+      </c>
+      <c r="F58">
+        <f t="shared" si="3"/>
+        <v>2.375</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>32</v>
+      </c>
+      <c r="B59">
+        <v>30</v>
+      </c>
+      <c r="C59">
+        <f t="shared" si="2"/>
+        <v>15.5</v>
+      </c>
+      <c r="D59">
+        <v>32</v>
+      </c>
+      <c r="E59">
+        <v>0</v>
+      </c>
+      <c r="F59">
+        <f t="shared" si="3"/>
+        <v>2.375</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>32</v>
+      </c>
+      <c r="B60">
+        <v>31</v>
+      </c>
+      <c r="C60">
+        <f t="shared" si="2"/>
+        <v>15.5</v>
+      </c>
+      <c r="D60">
+        <v>32</v>
+      </c>
+      <c r="E60">
+        <v>2</v>
+      </c>
+      <c r="F60">
+        <f t="shared" si="3"/>
+        <v>2.375</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
clearer graph fig 7
</commit_message>
<xml_diff>
--- a/doc/diag/finger_performance.xlsx
+++ b/doc/diag/finger_performance.xlsx
@@ -84,10 +84,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -149,8 +149,8 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
+            <c:symbol val="star"/>
+            <c:size val="6"/>
             <c:spPr>
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
@@ -234,11 +234,17 @@
               </a:solidFill>
               <a:round/>
             </a:ln>
-            <a:effectLst/>
+            <a:effectLst>
+              <a:glow>
+                <a:schemeClr val="accent1">
+                  <a:alpha val="40000"/>
+                </a:schemeClr>
+              </a:glow>
+            </a:effectLst>
           </c:spPr>
           <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
+            <c:symbol val="triangle"/>
+            <c:size val="6"/>
             <c:spPr>
               <a:solidFill>
                 <a:schemeClr val="accent2"/>
@@ -248,7 +254,13 @@
                   <a:schemeClr val="accent2"/>
                 </a:solidFill>
               </a:ln>
-              <a:effectLst/>
+              <a:effectLst>
+                <a:glow>
+                  <a:schemeClr val="accent1">
+                    <a:alpha val="40000"/>
+                  </a:schemeClr>
+                </a:glow>
+              </a:effectLst>
             </c:spPr>
           </c:marker>
           <c:cat>
@@ -311,11 +323,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1557282592"/>
-        <c:axId val="1557285856"/>
+        <c:axId val="-1419401392"/>
+        <c:axId val="-1419399760"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1557282592"/>
+        <c:axId val="-1419401392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -414,7 +426,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1557285856"/>
+        <c:crossAx val="-1419399760"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -422,7 +434,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1557285856"/>
+        <c:axId val="-1419399760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -529,7 +541,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1557282592"/>
+        <c:crossAx val="-1419401392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1501,7 +1513,7 @@
   <dimension ref="A1:M60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V33" sqref="V33"/>
+      <selection activeCell="U32" sqref="U32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1512,24 +1524,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2" t="s">
+      <c r="A1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="J1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="K1" s="3" t="s">
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="J1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="K1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -2903,16 +2915,16 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2" t="s">
+      <c r="A1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">

</xml_diff>

<commit_message>
log n to graph?
</commit_message>
<xml_diff>
--- a/doc/diag/finger_performance.xlsx
+++ b/doc/diag/finger_performance.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="7">
   <si>
     <t>nodes</t>
   </si>
@@ -44,6 +44,9 @@
   </si>
   <si>
     <t>ave</t>
+  </si>
+  <si>
+    <t>log(n)</t>
   </si>
 </sst>
 </file>
@@ -79,12 +82,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -94,6 +100,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF4BD0FF"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -142,7 +153,7 @@
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:srgbClr val="4BD0FF"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -153,11 +164,11 @@
             <c:size val="6"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:srgbClr val="4BD0FF"/>
               </a:solidFill>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:schemeClr val="accent1"/>
+                  <a:srgbClr val="4BD0FF"/>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
@@ -230,7 +241,7 @@
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent2"/>
+                <a:srgbClr val="FF0000"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -247,11 +258,11 @@
             <c:size val="6"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent2"/>
+                <a:srgbClr val="FF0000"/>
               </a:solidFill>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:schemeClr val="accent2"/>
+                  <a:srgbClr val="FF0000"/>
                 </a:solidFill>
               </a:ln>
               <a:effectLst>
@@ -313,6 +324,70 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$L$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>log(n)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$L$2:$L$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.4036774610288021</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
@@ -323,11 +398,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-1419401392"/>
-        <c:axId val="-1419399760"/>
+        <c:axId val="-975260656"/>
+        <c:axId val="-975262288"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1419401392"/>
+        <c:axId val="-975260656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -426,7 +501,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1419399760"/>
+        <c:crossAx val="-975262288"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -434,7 +509,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1419399760"/>
+        <c:axId val="-975262288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -541,7 +616,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1419401392"/>
+        <c:crossAx val="-975260656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -561,8 +636,8 @@
           <c:yMode val="edge"/>
           <c:x val="0.25867479099172552"/>
           <c:y val="0.93867221142811696"/>
-          <c:w val="0.48265041801654895"/>
-          <c:h val="4.9783777027871519E-2"/>
+          <c:w val="0.46565490186621006"/>
+          <c:h val="4.3689617268890299E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -1179,14 +1254,14 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>2</xdr:row>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>1</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>22</xdr:col>
-      <xdr:colOff>161925</xdr:colOff>
-      <xdr:row>28</xdr:row>
+      <xdr:colOff>409575</xdr:colOff>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>1</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1513,34 +1588,34 @@
   <dimension ref="A1:M60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U32" sqref="U32"/>
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="10" max="10" width="13.42578125" customWidth="1"/>
-    <col min="11" max="11" width="16.85546875" customWidth="1"/>
-    <col min="12" max="12" width="10.140625" customWidth="1"/>
+    <col min="10" max="12" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3" t="s">
+      <c r="A1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="J1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="K1" s="2" t="s">
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="J1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="K1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="L1" s="2"/>
+      <c r="L1" s="3" t="s">
+        <v>6</v>
+      </c>
       <c r="M1" s="2"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -1573,6 +1648,10 @@
         <f>VLOOKUP(I2,$D$3:$F$100,3,FALSE)</f>
         <v>0</v>
       </c>
+      <c r="L2">
+        <f>LOG(I2,4)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3">
@@ -1606,6 +1685,10 @@
         <f t="shared" ref="K3:K6" si="1">VLOOKUP(I3,$D$3:$F$100,3,FALSE)</f>
         <v>0.5</v>
       </c>
+      <c r="L3">
+        <f t="shared" ref="L3:L6" si="2">LOG(I3,4)</f>
+        <v>0.5</v>
+      </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4">
@@ -1615,7 +1698,7 @@
         <v>1</v>
       </c>
       <c r="C4">
-        <f t="shared" ref="C4:C60" si="2">AVERAGEIF($A$3:$A$100,A4,$B$3:$B$100)</f>
+        <f t="shared" ref="C4:C60" si="3">AVERAGEIF($A$3:$A$100,A4,$B$3:$B$100)</f>
         <v>3</v>
       </c>
       <c r="D4">
@@ -1625,7 +1708,7 @@
         <v>1</v>
       </c>
       <c r="F4">
-        <f t="shared" ref="F4:F60" si="3">AVERAGEIF($D$3:$D$100,D4,$E$3:$E$100)</f>
+        <f t="shared" ref="F4:F60" si="4">AVERAGEIF($D$3:$D$100,D4,$E$3:$E$100)</f>
         <v>1</v>
       </c>
       <c r="I4">
@@ -1638,6 +1721,10 @@
       <c r="K4">
         <f t="shared" si="1"/>
         <v>1</v>
+      </c>
+      <c r="L4">
+        <f t="shared" si="2"/>
+        <v>1.4036774610288021</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -1648,7 +1735,7 @@
         <v>2</v>
       </c>
       <c r="C5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="D5">
@@ -1658,7 +1745,7 @@
         <v>1</v>
       </c>
       <c r="F5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="I5">
@@ -1672,6 +1759,10 @@
         <f t="shared" si="1"/>
         <v>1.75</v>
       </c>
+      <c r="L5">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6">
@@ -1681,7 +1772,7 @@
         <v>3</v>
       </c>
       <c r="C6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="D6">
@@ -1691,7 +1782,7 @@
         <v>1</v>
       </c>
       <c r="F6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="I6">
@@ -1705,6 +1796,10 @@
         <f t="shared" si="1"/>
         <v>2.375</v>
       </c>
+      <c r="L6">
+        <f t="shared" si="2"/>
+        <v>2.5</v>
+      </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7">
@@ -1714,7 +1809,7 @@
         <v>4</v>
       </c>
       <c r="C7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="D7">
@@ -1724,7 +1819,7 @@
         <v>0</v>
       </c>
       <c r="F7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -1736,7 +1831,7 @@
         <v>5</v>
       </c>
       <c r="C8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="D8">
@@ -1746,7 +1841,7 @@
         <v>1</v>
       </c>
       <c r="F8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -1758,7 +1853,7 @@
         <v>6</v>
       </c>
       <c r="C9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="D9">
@@ -1768,7 +1863,7 @@
         <v>2</v>
       </c>
       <c r="F9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -1780,7 +1875,7 @@
         <v>0</v>
       </c>
       <c r="C10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="D10">
@@ -1790,7 +1885,7 @@
         <v>0</v>
       </c>
       <c r="F10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -1802,7 +1897,7 @@
         <v>1</v>
       </c>
       <c r="C11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
       <c r="D11">
@@ -1812,7 +1907,7 @@
         <v>1</v>
       </c>
       <c r="F11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.5</v>
       </c>
     </row>
@@ -1824,7 +1919,7 @@
         <v>0</v>
       </c>
       <c r="C12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
       <c r="D12">
@@ -1834,7 +1929,7 @@
         <v>0</v>
       </c>
       <c r="F12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.5</v>
       </c>
     </row>
@@ -1846,7 +1941,7 @@
         <v>0</v>
       </c>
       <c r="C13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>7.5</v>
       </c>
       <c r="D13">
@@ -1856,7 +1951,7 @@
         <v>2</v>
       </c>
       <c r="F13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.75</v>
       </c>
     </row>
@@ -1868,7 +1963,7 @@
         <v>1</v>
       </c>
       <c r="C14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>7.5</v>
       </c>
       <c r="D14">
@@ -1878,7 +1973,7 @@
         <v>3</v>
       </c>
       <c r="F14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.75</v>
       </c>
     </row>
@@ -1890,7 +1985,7 @@
         <v>2</v>
       </c>
       <c r="C15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>7.5</v>
       </c>
       <c r="D15">
@@ -1900,7 +1995,7 @@
         <v>1</v>
       </c>
       <c r="F15">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.75</v>
       </c>
     </row>
@@ -1912,7 +2007,7 @@
         <v>3</v>
       </c>
       <c r="C16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>7.5</v>
       </c>
       <c r="D16">
@@ -1922,11 +2017,11 @@
         <v>2</v>
       </c>
       <c r="F16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.75</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1934,7 +2029,7 @@
         <v>4</v>
       </c>
       <c r="C17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>7.5</v>
       </c>
       <c r="D17">
@@ -1944,11 +2039,11 @@
         <v>4</v>
       </c>
       <c r="F17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.75</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>16</v>
       </c>
@@ -1956,7 +2051,7 @@
         <v>5</v>
       </c>
       <c r="C18">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>7.5</v>
       </c>
       <c r="D18">
@@ -1966,11 +2061,11 @@
         <v>2</v>
       </c>
       <c r="F18">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.75</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>16</v>
       </c>
@@ -1978,7 +2073,7 @@
         <v>6</v>
       </c>
       <c r="C19">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>7.5</v>
       </c>
       <c r="D19">
@@ -1988,11 +2083,11 @@
         <v>2</v>
       </c>
       <c r="F19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.75</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>16</v>
       </c>
@@ -2000,7 +2095,7 @@
         <v>7</v>
       </c>
       <c r="C20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>7.5</v>
       </c>
       <c r="D20">
@@ -2010,11 +2105,11 @@
         <v>2</v>
       </c>
       <c r="F20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.75</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>16</v>
       </c>
@@ -2022,7 +2117,7 @@
         <v>8</v>
       </c>
       <c r="C21">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>7.5</v>
       </c>
       <c r="D21">
@@ -2032,11 +2127,11 @@
         <v>1</v>
       </c>
       <c r="F21">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.75</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>16</v>
       </c>
@@ -2044,7 +2139,7 @@
         <v>9</v>
       </c>
       <c r="C22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>7.5</v>
       </c>
       <c r="D22">
@@ -2054,11 +2149,11 @@
         <v>1</v>
       </c>
       <c r="F22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.75</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>16</v>
       </c>
@@ -2066,7 +2161,7 @@
         <v>10</v>
       </c>
       <c r="C23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>7.5</v>
       </c>
       <c r="D23">
@@ -2076,11 +2171,11 @@
         <v>1</v>
       </c>
       <c r="F23">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.75</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>16</v>
       </c>
@@ -2088,7 +2183,7 @@
         <v>11</v>
       </c>
       <c r="C24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>7.5</v>
       </c>
       <c r="D24">
@@ -2098,11 +2193,11 @@
         <v>2</v>
       </c>
       <c r="F24">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.75</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>16</v>
       </c>
@@ -2110,7 +2205,7 @@
         <v>12</v>
       </c>
       <c r="C25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>7.5</v>
       </c>
       <c r="D25">
@@ -2120,11 +2215,11 @@
         <v>2</v>
       </c>
       <c r="F25">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.75</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>16</v>
       </c>
@@ -2132,7 +2227,7 @@
         <v>13</v>
       </c>
       <c r="C26">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>7.5</v>
       </c>
       <c r="D26">
@@ -2142,11 +2237,11 @@
         <v>1</v>
       </c>
       <c r="F26">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.75</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>16</v>
       </c>
@@ -2154,7 +2249,7 @@
         <v>14</v>
       </c>
       <c r="C27">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>7.5</v>
       </c>
       <c r="D27">
@@ -2164,11 +2259,11 @@
         <v>0</v>
       </c>
       <c r="F27">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.75</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>16</v>
       </c>
@@ -2176,7 +2271,7 @@
         <v>15</v>
       </c>
       <c r="C28">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>7.5</v>
       </c>
       <c r="D28">
@@ -2186,11 +2281,11 @@
         <v>2</v>
       </c>
       <c r="F28">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.75</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>32</v>
       </c>
@@ -2198,7 +2293,7 @@
         <v>0</v>
       </c>
       <c r="C29">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>15.5</v>
       </c>
       <c r="D29">
@@ -2208,11 +2303,11 @@
         <v>3</v>
       </c>
       <c r="F29">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2.375</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>32</v>
       </c>
@@ -2220,7 +2315,7 @@
         <v>1</v>
       </c>
       <c r="C30">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>15.5</v>
       </c>
       <c r="D30">
@@ -2230,11 +2325,11 @@
         <v>3</v>
       </c>
       <c r="F30">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2.375</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>32</v>
       </c>
@@ -2242,7 +2337,7 @@
         <v>2</v>
       </c>
       <c r="C31">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>15.5</v>
       </c>
       <c r="D31">
@@ -2252,11 +2347,26 @@
         <v>2</v>
       </c>
       <c r="F31">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2.375</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I31">
+        <v>1000</v>
+      </c>
+      <c r="J31">
+        <f>LOG($I$31)</f>
+        <v>3</v>
+      </c>
+      <c r="K31">
+        <f>LOG($I$31,POWER(2,4))</f>
+        <v>2.4914460711655217</v>
+      </c>
+      <c r="L31">
+        <f>LOG($I$31,10)</f>
+        <v>2.9999999999999996</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>32</v>
       </c>
@@ -2264,7 +2374,7 @@
         <v>3</v>
       </c>
       <c r="C32">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>15.5</v>
       </c>
       <c r="D32">
@@ -2274,8 +2384,12 @@
         <v>4</v>
       </c>
       <c r="F32">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2.375</v>
+      </c>
+      <c r="K32">
+        <f>POWER(2,4)</f>
+        <v>16</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -2286,7 +2400,7 @@
         <v>4</v>
       </c>
       <c r="C33">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>15.5</v>
       </c>
       <c r="D33">
@@ -2296,7 +2410,7 @@
         <v>2</v>
       </c>
       <c r="F33">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2.375</v>
       </c>
     </row>
@@ -2308,7 +2422,7 @@
         <v>5</v>
       </c>
       <c r="C34">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>15.5</v>
       </c>
       <c r="D34">
@@ -2318,7 +2432,7 @@
         <v>2</v>
       </c>
       <c r="F34">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2.375</v>
       </c>
     </row>
@@ -2330,7 +2444,7 @@
         <v>6</v>
       </c>
       <c r="C35">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>15.5</v>
       </c>
       <c r="D35">
@@ -2340,7 +2454,7 @@
         <v>2</v>
       </c>
       <c r="F35">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2.375</v>
       </c>
     </row>
@@ -2352,7 +2466,7 @@
         <v>7</v>
       </c>
       <c r="C36">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>15.5</v>
       </c>
       <c r="D36">
@@ -2362,7 +2476,7 @@
         <v>2</v>
       </c>
       <c r="F36">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2.375</v>
       </c>
     </row>
@@ -2374,7 +2488,7 @@
         <v>8</v>
       </c>
       <c r="C37">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>15.5</v>
       </c>
       <c r="D37">
@@ -2384,7 +2498,7 @@
         <v>3</v>
       </c>
       <c r="F37">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2.375</v>
       </c>
     </row>
@@ -2396,7 +2510,7 @@
         <v>9</v>
       </c>
       <c r="C38">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>15.5</v>
       </c>
       <c r="D38">
@@ -2406,7 +2520,7 @@
         <v>1</v>
       </c>
       <c r="F38">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2.375</v>
       </c>
     </row>
@@ -2418,7 +2532,7 @@
         <v>10</v>
       </c>
       <c r="C39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>15.5</v>
       </c>
       <c r="D39">
@@ -2428,7 +2542,7 @@
         <v>2</v>
       </c>
       <c r="F39">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2.375</v>
       </c>
     </row>
@@ -2440,7 +2554,7 @@
         <v>11</v>
       </c>
       <c r="C40">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>15.5</v>
       </c>
       <c r="D40">
@@ -2450,7 +2564,7 @@
         <v>3</v>
       </c>
       <c r="F40">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2.375</v>
       </c>
     </row>
@@ -2462,7 +2576,7 @@
         <v>12</v>
       </c>
       <c r="C41">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>15.5</v>
       </c>
       <c r="D41">
@@ -2472,7 +2586,7 @@
         <v>3</v>
       </c>
       <c r="F41">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2.375</v>
       </c>
     </row>
@@ -2484,7 +2598,7 @@
         <v>13</v>
       </c>
       <c r="C42">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>15.5</v>
       </c>
       <c r="D42">
@@ -2494,7 +2608,7 @@
         <v>2</v>
       </c>
       <c r="F42">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2.375</v>
       </c>
     </row>
@@ -2506,7 +2620,7 @@
         <v>14</v>
       </c>
       <c r="C43">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>15.5</v>
       </c>
       <c r="D43">
@@ -2516,7 +2630,7 @@
         <v>2</v>
       </c>
       <c r="F43">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2.375</v>
       </c>
     </row>
@@ -2528,7 +2642,7 @@
         <v>15</v>
       </c>
       <c r="C44">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>15.5</v>
       </c>
       <c r="D44">
@@ -2538,7 +2652,7 @@
         <v>3</v>
       </c>
       <c r="F44">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2.375</v>
       </c>
     </row>
@@ -2550,7 +2664,7 @@
         <v>16</v>
       </c>
       <c r="C45">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>15.5</v>
       </c>
       <c r="D45">
@@ -2560,7 +2674,7 @@
         <v>3</v>
       </c>
       <c r="F45">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2.375</v>
       </c>
     </row>
@@ -2572,7 +2686,7 @@
         <v>17</v>
       </c>
       <c r="C46">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>15.5</v>
       </c>
       <c r="D46">
@@ -2582,7 +2696,7 @@
         <v>3</v>
       </c>
       <c r="F46">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2.375</v>
       </c>
     </row>
@@ -2594,7 +2708,7 @@
         <v>18</v>
       </c>
       <c r="C47">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>15.5</v>
       </c>
       <c r="D47">
@@ -2604,7 +2718,7 @@
         <v>1</v>
       </c>
       <c r="F47">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2.375</v>
       </c>
     </row>
@@ -2616,7 +2730,7 @@
         <v>19</v>
       </c>
       <c r="C48">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>15.5</v>
       </c>
       <c r="D48">
@@ -2626,7 +2740,7 @@
         <v>1</v>
       </c>
       <c r="F48">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2.375</v>
       </c>
     </row>
@@ -2638,7 +2752,7 @@
         <v>20</v>
       </c>
       <c r="C49">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>15.5</v>
       </c>
       <c r="D49">
@@ -2648,7 +2762,7 @@
         <v>3</v>
       </c>
       <c r="F49">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2.375</v>
       </c>
     </row>
@@ -2660,7 +2774,7 @@
         <v>21</v>
       </c>
       <c r="C50">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>15.5</v>
       </c>
       <c r="D50">
@@ -2670,7 +2784,7 @@
         <v>2</v>
       </c>
       <c r="F50">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2.375</v>
       </c>
     </row>
@@ -2682,7 +2796,7 @@
         <v>22</v>
       </c>
       <c r="C51">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>15.5</v>
       </c>
       <c r="D51">
@@ -2692,7 +2806,7 @@
         <v>3</v>
       </c>
       <c r="F51">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2.375</v>
       </c>
     </row>
@@ -2704,7 +2818,7 @@
         <v>23</v>
       </c>
       <c r="C52">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>15.5</v>
       </c>
       <c r="D52">
@@ -2714,7 +2828,7 @@
         <v>2</v>
       </c>
       <c r="F52">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2.375</v>
       </c>
     </row>
@@ -2726,7 +2840,7 @@
         <v>24</v>
       </c>
       <c r="C53">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>15.5</v>
       </c>
       <c r="D53">
@@ -2736,7 +2850,7 @@
         <v>3</v>
       </c>
       <c r="F53">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2.375</v>
       </c>
     </row>
@@ -2748,7 +2862,7 @@
         <v>25</v>
       </c>
       <c r="C54">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>15.5</v>
       </c>
       <c r="D54">
@@ -2758,7 +2872,7 @@
         <v>2</v>
       </c>
       <c r="F54">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2.375</v>
       </c>
     </row>
@@ -2770,7 +2884,7 @@
         <v>26</v>
       </c>
       <c r="C55">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>15.5</v>
       </c>
       <c r="D55">
@@ -2780,7 +2894,7 @@
         <v>3</v>
       </c>
       <c r="F55">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2.375</v>
       </c>
     </row>
@@ -2792,7 +2906,7 @@
         <v>27</v>
       </c>
       <c r="C56">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>15.5</v>
       </c>
       <c r="D56">
@@ -2802,7 +2916,7 @@
         <v>3</v>
       </c>
       <c r="F56">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2.375</v>
       </c>
     </row>
@@ -2814,7 +2928,7 @@
         <v>28</v>
       </c>
       <c r="C57">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>15.5</v>
       </c>
       <c r="D57">
@@ -2824,7 +2938,7 @@
         <v>3</v>
       </c>
       <c r="F57">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2.375</v>
       </c>
     </row>
@@ -2836,7 +2950,7 @@
         <v>29</v>
       </c>
       <c r="C58">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>15.5</v>
       </c>
       <c r="D58">
@@ -2846,7 +2960,7 @@
         <v>3</v>
       </c>
       <c r="F58">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2.375</v>
       </c>
     </row>
@@ -2858,7 +2972,7 @@
         <v>30</v>
       </c>
       <c r="C59">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>15.5</v>
       </c>
       <c r="D59">
@@ -2868,7 +2982,7 @@
         <v>0</v>
       </c>
       <c r="F59">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2.375</v>
       </c>
     </row>
@@ -2880,7 +2994,7 @@
         <v>31</v>
       </c>
       <c r="C60">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>15.5</v>
       </c>
       <c r="D60">
@@ -2890,7 +3004,7 @@
         <v>2</v>
       </c>
       <c r="F60">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2.375</v>
       </c>
     </row>
@@ -2915,16 +3029,16 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3" t="s">
+      <c r="A1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">

</xml_diff>